<commit_message>
Auto stash before merge of "francisco-release" and "origin/wall-of-death/v1.0"
</commit_message>
<xml_diff>
--- a/backend/upload/test_file.xlsx
+++ b/backend/upload/test_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximo Hernandez\Documents\Repositorios\SoftProyectAdmin_G4\backend\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xpach\OneDrive\Desktop\SoftProyectAdmin_G4-master\backend\xlsx_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F94BD-9526-4C84-9363-487DA067BF8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98405426-7732-4F82-9CA8-2C8AC1869291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,34 +34,13 @@
     <t>Número de ID</t>
   </si>
   <si>
-    <t>Maximo</t>
-  </si>
-  <si>
-    <t>Hernandez</t>
-  </si>
-  <si>
-    <t>mahernandez15@alumnos.utalca.cl</t>
-  </si>
-  <si>
-    <t>Pepe</t>
-  </si>
-  <si>
-    <t>Diaz</t>
-  </si>
-  <si>
-    <t>pdiaz@utalca.cl</t>
-  </si>
-  <si>
-    <t>Ele</t>
-  </si>
-  <si>
-    <t>Mental</t>
-  </si>
-  <si>
-    <t>elmental21@alumnos.utalca.cl</t>
-  </si>
-  <si>
-    <t>elmental221@alumnos.utalca.cl</t>
+    <t>n8</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>c8@alumnos.utalca.cl</t>
   </si>
 </sst>
 </file>
@@ -82,10 +61,10 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,16 +84,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,15 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,69 +429,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" s="1"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F133FC5A-7B2E-4BC3-9964-804E8AC09ED5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>